<commit_message>
Fixed another fuck up
</commit_message>
<xml_diff>
--- a/aging.xlsx
+++ b/aging.xlsx
@@ -14,35 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>PSU</t>
   </si>
   <si>
-    <t>PET</t>
-  </si>
-  <si>
-    <t>Nylon-6_exp2</t>
-  </si>
-  <si>
-    <t>Nylon-6_exp2 2.1</t>
-  </si>
-  <si>
-    <t>Nylon-6_exp2 2.2</t>
-  </si>
-  <si>
-    <t>Nylon-6_exp2 2.3</t>
-  </si>
-  <si>
-    <t>PET S1</t>
-  </si>
-  <si>
-    <t>PET S2</t>
-  </si>
-  <si>
-    <t>PET S3</t>
-  </si>
-  <si>
     <t>PSU S1</t>
   </si>
   <si>
@@ -52,31 +28,13 @@
     <t>PSU S3</t>
   </si>
   <si>
-    <t>{0.0: 2408.8682766109705}</t>
-  </si>
-  <si>
-    <t>{0.0: 2249.0969300679862}</t>
-  </si>
-  <si>
-    <t>{0.0: 2213.7928614257835}</t>
-  </si>
-  <si>
-    <t>{0.0: 2596.1042148899287}</t>
-  </si>
-  <si>
-    <t>{0.0: 2526.8181263750885}</t>
-  </si>
-  <si>
-    <t>{0.0: 2563.316223674454}</t>
-  </si>
-  <si>
-    <t>{0.0: 2436.757677510963}</t>
-  </si>
-  <si>
-    <t>{0.0: 2510.7010696167126}</t>
-  </si>
-  <si>
-    <t>{0.0: 2725.396147437743}</t>
+    <t>{0.0: 2494.9877810440958}</t>
+  </si>
+  <si>
+    <t>{0.0: 2430.1591997439973}</t>
+  </si>
+  <si>
+    <t>{0.0: 2330.071670255158}</t>
   </si>
 </sst>
 </file>
@@ -434,93 +392,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>